<commit_message>
Actualizar hoja Avatares en el Excel
</commit_message>
<xml_diff>
--- a/Base_Asistente_Imagenes_Estructuradas.xlsx
+++ b/Base_Asistente_Imagenes_Estructuradas.xlsx
@@ -1,16 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28801"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{75FB986F-1C45-4DEA-A185-E8C09594A15C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Clientes" sheetId="1" r:id="rId1"/>
+    <sheet name="Avatares" sheetId="1" r:id="rId1"/>
     <sheet name="Prendas" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="191028"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -80,300 +97,300 @@
     <t>CL1</t>
   </si>
   <si>
+    <t>Sofía</t>
+  </si>
+  <si>
+    <t>Martínez</t>
+  </si>
+  <si>
+    <t>Mujer</t>
+  </si>
+  <si>
+    <t>adolfo.montero@gmail.com</t>
+  </si>
+  <si>
+    <t>Valencia</t>
+  </si>
+  <si>
+    <t>Minimalista</t>
+  </si>
+  <si>
+    <t>XL</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/tMioNwn.png</t>
+  </si>
+  <si>
+    <t>Cena</t>
+  </si>
+  <si>
+    <t>Sí</t>
+  </si>
+  <si>
+    <t>Vaqueros rectos</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>P06</t>
+  </si>
+  <si>
+    <t>Avatar_Sofía_Martínez_CL1_seed8821</t>
+  </si>
+  <si>
     <t>CL2</t>
   </si>
   <si>
+    <t>Jaime</t>
+  </si>
+  <si>
+    <t>Madrigal Espada</t>
+  </si>
+  <si>
+    <t>Hombre</t>
+  </si>
+  <si>
+    <t>amontero@icloud.com</t>
+  </si>
+  <si>
+    <t>Álava</t>
+  </si>
+  <si>
+    <t>Moderno</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/fHAoKJt.png</t>
+  </si>
+  <si>
+    <t>Cita</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>Avatar_Jaime_Madrigal_Espada_CL2_seed1160</t>
+  </si>
+  <si>
     <t>CL3</t>
   </si>
   <si>
+    <t>Santiago</t>
+  </si>
+  <si>
+    <t>Lastra Badía</t>
+  </si>
+  <si>
+    <t>lroldan@andina.es</t>
+  </si>
+  <si>
+    <t>Urbano</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/p9Jm9rJ.png</t>
+  </si>
+  <si>
+    <t>Polo algodón piqué</t>
+  </si>
+  <si>
+    <t>P17</t>
+  </si>
+  <si>
+    <t>Avatar_Santiago_Lastra_Badía_CL3_seed7815</t>
+  </si>
+  <si>
     <t>CL4</t>
   </si>
   <si>
+    <t>Julia</t>
+  </si>
+  <si>
+    <t>López</t>
+  </si>
+  <si>
+    <t>jullóp16@andina.es</t>
+  </si>
+  <si>
+    <t>Cantabria</t>
+  </si>
+  <si>
+    <t>Romántico</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/oTtPndH.png</t>
+  </si>
+  <si>
+    <t>Día casual</t>
+  </si>
+  <si>
+    <t>Sudadera oversize negra</t>
+  </si>
+  <si>
+    <t>P09</t>
+  </si>
+  <si>
+    <t>Avatar_Julia_López_CL4_seed2402</t>
+  </si>
+  <si>
     <t>CL5</t>
   </si>
   <si>
+    <t>Carmen</t>
+  </si>
+  <si>
+    <t>Alonso</t>
+  </si>
+  <si>
+    <t>caralo19@andina.es</t>
+  </si>
+  <si>
+    <t>Segovia</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/i8m3xgd.png</t>
+  </si>
+  <si>
+    <t>Evento especial</t>
+  </si>
+  <si>
+    <t>Jersey cuello alto gris</t>
+  </si>
+  <si>
+    <t>P14</t>
+  </si>
+  <si>
+    <t>Avatar_Carmen_Alonso_CL5_seed3079</t>
+  </si>
+  <si>
     <t>CL6</t>
   </si>
   <si>
+    <t>Valeria</t>
+  </si>
+  <si>
+    <t>Navas</t>
+  </si>
+  <si>
+    <t>valnav36@andina.es</t>
+  </si>
+  <si>
+    <t>Soria</t>
+  </si>
+  <si>
+    <t>Elegante</t>
+  </si>
+  <si>
+    <t>XS</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/Y6GCixv.png</t>
+  </si>
+  <si>
+    <t>Fin de semana</t>
+  </si>
+  <si>
+    <t>Camisa lino blanca</t>
+  </si>
+  <si>
+    <t>Avatar_Valeria_Navas_CL6_seed6037</t>
+  </si>
+  <si>
     <t>CL7</t>
   </si>
   <si>
+    <t>Laura</t>
+  </si>
+  <si>
+    <t>García</t>
+  </si>
+  <si>
+    <t>laugar85@andina.es</t>
+  </si>
+  <si>
+    <t>Guipúzcoa</t>
+  </si>
+  <si>
+    <t>Glam</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/NNh64T7.png</t>
+  </si>
+  <si>
+    <t>Pantalón cargo beige</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>Avatar_Laura_García_CL7_seed8723</t>
+  </si>
+  <si>
     <t>CL8</t>
   </si>
   <si>
+    <t>Andrés</t>
+  </si>
+  <si>
+    <t>Chacón Mateos</t>
+  </si>
+  <si>
+    <t>lorenza42@andina.es</t>
+  </si>
+  <si>
+    <t>Castellón</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/7xcV9Vq.png</t>
+  </si>
+  <si>
+    <t>Avatar_Andrés_Chacón_Mateos_CL8_seed8821</t>
+  </si>
+  <si>
     <t>CL9</t>
   </si>
   <si>
+    <t>Damián</t>
+  </si>
+  <si>
+    <t>Zurita</t>
+  </si>
+  <si>
+    <t>galvezsandra@andina.es</t>
+  </si>
+  <si>
+    <t>Teruel</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/CVpVkfy.png</t>
+  </si>
+  <si>
+    <t>Avatar_Damián_Zurita_CL9_seed1817</t>
+  </si>
+  <si>
     <t>CL10</t>
   </si>
   <si>
-    <t>Sofía</t>
-  </si>
-  <si>
-    <t>Jaime</t>
-  </si>
-  <si>
-    <t>Santiago</t>
-  </si>
-  <si>
-    <t>Julia</t>
-  </si>
-  <si>
-    <t>Carmen</t>
-  </si>
-  <si>
-    <t>Valeria</t>
-  </si>
-  <si>
-    <t>Laura</t>
-  </si>
-  <si>
-    <t>Andrés</t>
-  </si>
-  <si>
-    <t>Damián</t>
-  </si>
-  <si>
     <t>Ismael</t>
   </si>
   <si>
-    <t>Martínez</t>
-  </si>
-  <si>
-    <t>Madrigal Espada</t>
-  </si>
-  <si>
-    <t>Lastra Badía</t>
-  </si>
-  <si>
-    <t>López</t>
-  </si>
-  <si>
-    <t>Alonso</t>
-  </si>
-  <si>
-    <t>Navas</t>
-  </si>
-  <si>
-    <t>García</t>
-  </si>
-  <si>
-    <t>Chacón Mateos</t>
-  </si>
-  <si>
-    <t>Zurita</t>
-  </si>
-  <si>
     <t xml:space="preserve">Rosa </t>
   </si>
   <si>
-    <t>Mujer</t>
-  </si>
-  <si>
-    <t>Hombre</t>
-  </si>
-  <si>
-    <t>adolfo.montero@gmail.com</t>
-  </si>
-  <si>
-    <t>amontero@icloud.com</t>
-  </si>
-  <si>
-    <t>lroldan@andina.es</t>
-  </si>
-  <si>
-    <t>jullóp16@andina.es</t>
-  </si>
-  <si>
-    <t>caralo19@andina.es</t>
-  </si>
-  <si>
-    <t>valnav36@andina.es</t>
-  </si>
-  <si>
-    <t>laugar85@andina.es</t>
-  </si>
-  <si>
-    <t>lorenza42@andina.es</t>
-  </si>
-  <si>
-    <t>galvezsandra@andina.es</t>
-  </si>
-  <si>
     <t>valencianovalentina@andina.es</t>
   </si>
   <si>
-    <t>Valencia</t>
-  </si>
-  <si>
-    <t>Álava</t>
-  </si>
-  <si>
-    <t>Cantabria</t>
-  </si>
-  <si>
-    <t>Segovia</t>
-  </si>
-  <si>
-    <t>Soria</t>
-  </si>
-  <si>
-    <t>Guipúzcoa</t>
-  </si>
-  <si>
-    <t>Castellón</t>
-  </si>
-  <si>
-    <t>Teruel</t>
-  </si>
-  <si>
     <t>Ceuta</t>
   </si>
   <si>
-    <t>Minimalista</t>
-  </si>
-  <si>
-    <t>Moderno</t>
-  </si>
-  <si>
-    <t>Urbano</t>
-  </si>
-  <si>
-    <t>Romántico</t>
-  </si>
-  <si>
-    <t>Elegante</t>
-  </si>
-  <si>
-    <t>Glam</t>
-  </si>
-  <si>
-    <t>XL</t>
-  </si>
-  <si>
-    <t>S</t>
-  </si>
-  <si>
-    <t>M</t>
-  </si>
-  <si>
-    <t>XS</t>
-  </si>
-  <si>
-    <t>https://i.imgur.com/tMioNwn.png</t>
-  </si>
-  <si>
-    <t>https://i.imgur.com/fHAoKJt.png</t>
-  </si>
-  <si>
-    <t>https://i.imgur.com/p9Jm9rJ.png</t>
-  </si>
-  <si>
-    <t>https://i.imgur.com/oTtPndH.png</t>
-  </si>
-  <si>
-    <t>https://i.imgur.com/i8m3xgd.png</t>
-  </si>
-  <si>
-    <t>https://i.imgur.com/Y6GCixv.png</t>
-  </si>
-  <si>
-    <t>https://i.imgur.com/NNh64T7.png</t>
-  </si>
-  <si>
-    <t>https://i.imgur.com/7xcV9Vq.png</t>
-  </si>
-  <si>
-    <t>https://i.imgur.com/CVpVkfy.png</t>
-  </si>
-  <si>
     <t>https://i.imgur.com/R5CN6rY.png</t>
   </si>
   <si>
-    <t>Cena</t>
-  </si>
-  <si>
-    <t>Cita</t>
-  </si>
-  <si>
-    <t>Día casual</t>
-  </si>
-  <si>
-    <t>Evento especial</t>
-  </si>
-  <si>
-    <t>Fin de semana</t>
-  </si>
-  <si>
     <t>Trabajo</t>
   </si>
   <si>
-    <t>Sí</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>Vaqueros rectos</t>
-  </si>
-  <si>
-    <t>Polo algodón piqué</t>
-  </si>
-  <si>
-    <t>Sudadera oversize negra</t>
-  </si>
-  <si>
-    <t>Jersey cuello alto gris</t>
-  </si>
-  <si>
-    <t>Camisa lino blanca</t>
-  </si>
-  <si>
-    <t>Pantalón cargo beige</t>
-  </si>
-  <si>
-    <t>L</t>
-  </si>
-  <si>
-    <t>P06</t>
-  </si>
-  <si>
-    <t>P17</t>
-  </si>
-  <si>
-    <t>P09</t>
-  </si>
-  <si>
-    <t>P14</t>
-  </si>
-  <si>
-    <t>Avatar_Sofía_Martínez_CL1_seed8821</t>
-  </si>
-  <si>
-    <t>Avatar_Jaime_Madrigal_Espada_CL2_seed1160</t>
-  </si>
-  <si>
-    <t>Avatar_Santiago_Lastra_Badía_CL3_seed7815</t>
-  </si>
-  <si>
-    <t>Avatar_Julia_López_CL4_seed2402</t>
-  </si>
-  <si>
-    <t>Avatar_Carmen_Alonso_CL5_seed3079</t>
-  </si>
-  <si>
-    <t>Avatar_Valeria_Navas_CL6_seed6037</t>
-  </si>
-  <si>
-    <t>Avatar_Laura_García_CL7_seed8723</t>
-  </si>
-  <si>
-    <t>Avatar_Andrés_Chacón_Mateos_CL8_seed8821</t>
-  </si>
-  <si>
-    <t>Avatar_Damián_Zurita_CL9_seed1817</t>
-  </si>
-  <si>
     <t>Avatar_Ismael_Rosa_CL10_seed6053</t>
   </si>
   <si>
@@ -416,340 +433,340 @@
     <t>P01</t>
   </si>
   <si>
+    <t>Vestido camisero Blanco</t>
+  </si>
+  <si>
+    <t>Vestido camisero</t>
+  </si>
+  <si>
+    <t>Vestido</t>
+  </si>
+  <si>
+    <t>lino</t>
+  </si>
+  <si>
+    <t>Primavera/verano</t>
+  </si>
+  <si>
+    <t>['S', 'M', 'L']</t>
+  </si>
+  <si>
+    <t>100% lino</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/fHtxOlI.png</t>
+  </si>
+  <si>
+    <t>Prenda_Vestido_camisero_Vestido_camisero_Blanco_P01_seed4275</t>
+  </si>
+  <si>
     <t>P02</t>
   </si>
   <si>
+    <t>Pantalón palazzo Blanco</t>
+  </si>
+  <si>
+    <t>Pantalón palazzo</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/jUvfENS.png</t>
+  </si>
+  <si>
+    <t>Prenda_Pantalón_palazzo_Pantalón_palazzo_Blanco_P02_seed6692</t>
+  </si>
+  <si>
     <t>P03</t>
   </si>
   <si>
+    <t>Top Negro</t>
+  </si>
+  <si>
+    <t>Top</t>
+  </si>
+  <si>
+    <t>poliéster</t>
+  </si>
+  <si>
+    <t>Todo el año</t>
+  </si>
+  <si>
+    <t>['M', 'L', 'XL']</t>
+  </si>
+  <si>
+    <t>95% poliéster, 5% elastano</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/XM8Jr96.jpg</t>
+  </si>
+  <si>
+    <t>Prenda_Top_Top_Negro_P03_seed4206</t>
+  </si>
+  <si>
     <t>P04</t>
   </si>
   <si>
+    <t>Falda midi satinada Gris claro</t>
+  </si>
+  <si>
+    <t>Falda midi satinada</t>
+  </si>
+  <si>
+    <t>Falda</t>
+  </si>
+  <si>
+    <t>viscosa</t>
+  </si>
+  <si>
+    <t>Evento</t>
+  </si>
+  <si>
+    <t>70% viscosa, 30% lino</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/8aFsMDj.png</t>
+  </si>
+  <si>
+    <t>Prenda_Falda_midi_satinada_Falda_midi_satinada_Gris_claro_P04_seed2216</t>
+  </si>
+  <si>
     <t>P05</t>
   </si>
   <si>
+    <t>Falda midi satinada verde</t>
+  </si>
+  <si>
+    <t>Casual</t>
+  </si>
+  <si>
+    <t>Otoño/invierno</t>
+  </si>
+  <si>
+    <t>65% poliéster, 35% algodón</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/osm3SL1.png</t>
+  </si>
+  <si>
+    <t>Prenda_Falda_midi_satinada_Falda_midi_satinada_verde_P05_seed7292</t>
+  </si>
+  <si>
+    <t>Chaqueta de estilo Elegante en color Camel</t>
+  </si>
+  <si>
+    <t>Chaqueta</t>
+  </si>
+  <si>
+    <t>['XS', 'S', 'M']</t>
+  </si>
+  <si>
+    <t>68% lino, 37% algodón</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/d8NmBSD.png</t>
+  </si>
+  <si>
+    <t>Prenda_Chaqueta_Chaqueta_de_estilo_Elegante_en_color_Camel_P06_seed1474</t>
+  </si>
+  <si>
     <t>P07</t>
   </si>
   <si>
+    <t>Polo de estilo Elegante en color Azul</t>
+  </si>
+  <si>
+    <t>Polo</t>
+  </si>
+  <si>
+    <t>65% viscosa, 27% algodón</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/msRQCCY.png</t>
+  </si>
+  <si>
+    <t>Prenda_Polo_Polo_de_estilo_Elegante_en_color_Azul_P07_seed9180</t>
+  </si>
+  <si>
     <t>P08</t>
   </si>
   <si>
+    <t>Camisa de estilo Casual en color Beige</t>
+  </si>
+  <si>
+    <t>Camisa</t>
+  </si>
+  <si>
+    <t>Lino</t>
+  </si>
+  <si>
+    <t>64% viscosa, 24% algodón</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/dreKWca.png</t>
+  </si>
+  <si>
+    <t>Prenda_Camisa_Camisa_de_estilo_Casual_en_color_Beige_P08_seed8912</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Camiseta blanca </t>
+  </si>
+  <si>
+    <t>Camiseta</t>
+  </si>
+  <si>
+    <t>Algodón</t>
+  </si>
+  <si>
+    <t>100% algodón</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/k7fUFZv.png</t>
+  </si>
+  <si>
+    <t>Prenda_Camiseta_Camiseta_blanca_P09_seed5276</t>
+  </si>
+  <si>
     <t>P10</t>
   </si>
   <si>
+    <t>Chaqueta de estilo elegante ceñida Azul marino</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/TYBSLcw.jpg</t>
+  </si>
+  <si>
+    <t>Prenda_Chaqueta_Chaqueta_de_estilo_elegante_ceñida_Azul_marino_P10_seed3580</t>
+  </si>
+  <si>
     <t xml:space="preserve">P11 </t>
   </si>
   <si>
+    <t>Chaqueta vaquera</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/va7NeF3.png</t>
+  </si>
+  <si>
+    <t>Prenda_Chaqueta_Chaqueta_vaquera_P11 _seed3547</t>
+  </si>
+  <si>
     <t>P12</t>
   </si>
   <si>
+    <t>Pantalón</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pantalón </t>
+  </si>
+  <si>
+    <t>Deporte</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/sclH3wO.png</t>
+  </si>
+  <si>
+    <t>Prenda_Pantalón_Pantalón_P12_seed5786</t>
+  </si>
+  <si>
     <t>P13</t>
   </si>
   <si>
+    <t>Vaquero</t>
+  </si>
+  <si>
+    <t>Sport</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/Ay0SsXe.png</t>
+  </si>
+  <si>
+    <t>Prenda_Vaquero_Pantalón_P13_seed3420</t>
+  </si>
+  <si>
+    <t>Sudadera</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/OwL8OBA.png</t>
+  </si>
+  <si>
+    <t>Prenda_Sudadera_Sudadera_P14_seed7474</t>
+  </si>
+  <si>
     <t>P15</t>
   </si>
   <si>
+    <t>Vestido rojo</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/ARsYA1K.png</t>
+  </si>
+  <si>
+    <t>Prenda_Vestido_Vestido_rojo_P15_seed9029</t>
+  </si>
+  <si>
     <t>P16</t>
   </si>
   <si>
+    <t xml:space="preserve">Camisa Blanca </t>
+  </si>
+  <si>
+    <t>Traje</t>
+  </si>
+  <si>
+    <t>100% Algodón</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/G0MNOx2.png</t>
+  </si>
+  <si>
+    <t>Prenda_Camisa_Camisa_Blanca_P16_seed4304</t>
+  </si>
+  <si>
+    <t>Camisa marrón</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/JtJYtkX.jpg</t>
+  </si>
+  <si>
+    <t>Prenda_Camisa_Camisa_marrón_P17_seed8562</t>
+  </si>
+  <si>
     <t>P18</t>
   </si>
   <si>
+    <t>Pantalón Chino azul</t>
+  </si>
+  <si>
+    <t>Chino</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/xKONxAZ.png</t>
+  </si>
+  <si>
+    <t>Prenda_Pantalón_Pantalón_Chino_azul_P18_seed1907</t>
+  </si>
+  <si>
     <t>P19</t>
   </si>
   <si>
+    <t>Abrigo Largo verde</t>
+  </si>
+  <si>
+    <t>Abrigo</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/mQrejMN.jpg</t>
+  </si>
+  <si>
+    <t>Prenda_Abrigo_Abrigo_Largo_verde_P19_seed6232</t>
+  </si>
+  <si>
     <t>P20</t>
   </si>
   <si>
-    <t>Vestido camisero Blanco</t>
-  </si>
-  <si>
-    <t>Pantalón palazzo Blanco</t>
-  </si>
-  <si>
-    <t>Top Negro</t>
-  </si>
-  <si>
-    <t>Falda midi satinada Gris claro</t>
-  </si>
-  <si>
-    <t>Falda midi satinada verde</t>
-  </si>
-  <si>
-    <t>Chaqueta de estilo Elegante en color Camel</t>
-  </si>
-  <si>
-    <t>Polo de estilo Elegante en color Azul</t>
-  </si>
-  <si>
-    <t>Camisa de estilo Casual en color Beige</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Camiseta blanca </t>
-  </si>
-  <si>
-    <t>Chaqueta de estilo elegante ceñida Azul marino</t>
-  </si>
-  <si>
-    <t>Chaqueta vaquera</t>
-  </si>
-  <si>
-    <t>Pantalón</t>
-  </si>
-  <si>
-    <t>Sudadera</t>
-  </si>
-  <si>
-    <t>Vestido rojo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Camisa Blanca </t>
-  </si>
-  <si>
-    <t>Camisa marrón</t>
-  </si>
-  <si>
-    <t>Pantalón Chino azul</t>
-  </si>
-  <si>
-    <t>Abrigo Largo verde</t>
-  </si>
-  <si>
     <t>Pantalón verde</t>
   </si>
   <si>
-    <t>Vestido camisero</t>
-  </si>
-  <si>
-    <t>Pantalón palazzo</t>
-  </si>
-  <si>
-    <t>Top</t>
-  </si>
-  <si>
-    <t>Falda midi satinada</t>
-  </si>
-  <si>
-    <t>Chaqueta</t>
-  </si>
-  <si>
-    <t>Polo</t>
-  </si>
-  <si>
-    <t>Camisa</t>
-  </si>
-  <si>
-    <t>Camiseta</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pantalón </t>
-  </si>
-  <si>
-    <t>Vaquero</t>
-  </si>
-  <si>
-    <t>Vestido</t>
-  </si>
-  <si>
-    <t>Abrigo</t>
-  </si>
-  <si>
-    <t>Falda</t>
-  </si>
-  <si>
-    <t>Deporte</t>
-  </si>
-  <si>
-    <t>Sport</t>
-  </si>
-  <si>
-    <t>Traje</t>
-  </si>
-  <si>
-    <t>Chino</t>
-  </si>
-  <si>
-    <t>Casual</t>
-  </si>
-  <si>
-    <t>lino</t>
-  </si>
-  <si>
-    <t>poliéster</t>
-  </si>
-  <si>
-    <t>viscosa</t>
-  </si>
-  <si>
-    <t>Lino</t>
-  </si>
-  <si>
-    <t>Algodón</t>
-  </si>
-  <si>
-    <t>Primavera/verano</t>
-  </si>
-  <si>
-    <t>Todo el año</t>
-  </si>
-  <si>
-    <t>Otoño/invierno</t>
-  </si>
-  <si>
-    <t>Evento</t>
-  </si>
-  <si>
-    <t>['S', 'M', 'L']</t>
-  </si>
-  <si>
-    <t>['M', 'L', 'XL']</t>
-  </si>
-  <si>
-    <t>['XS', 'S', 'M']</t>
-  </si>
-  <si>
-    <t>100% lino</t>
-  </si>
-  <si>
-    <t>95% poliéster, 5% elastano</t>
-  </si>
-  <si>
-    <t>70% viscosa, 30% lino</t>
-  </si>
-  <si>
-    <t>65% poliéster, 35% algodón</t>
-  </si>
-  <si>
-    <t>68% lino, 37% algodón</t>
-  </si>
-  <si>
-    <t>65% viscosa, 27% algodón</t>
-  </si>
-  <si>
-    <t>64% viscosa, 24% algodón</t>
-  </si>
-  <si>
-    <t>100% algodón</t>
-  </si>
-  <si>
-    <t>100% Algodón</t>
-  </si>
-  <si>
-    <t>https://i.imgur.com/fHtxOlI.png</t>
-  </si>
-  <si>
-    <t>https://i.imgur.com/jUvfENS.png</t>
-  </si>
-  <si>
-    <t>https://i.imgur.com/XM8Jr96.jpg</t>
-  </si>
-  <si>
-    <t>https://i.imgur.com/8aFsMDj.png</t>
-  </si>
-  <si>
-    <t>https://i.imgur.com/osm3SL1.png</t>
-  </si>
-  <si>
-    <t>https://i.imgur.com/d8NmBSD.png</t>
-  </si>
-  <si>
-    <t>https://i.imgur.com/msRQCCY.png</t>
-  </si>
-  <si>
-    <t>https://i.imgur.com/dreKWca.png</t>
-  </si>
-  <si>
-    <t>https://i.imgur.com/k7fUFZv.png</t>
-  </si>
-  <si>
-    <t>https://i.imgur.com/TYBSLcw.jpg</t>
-  </si>
-  <si>
-    <t>https://i.imgur.com/va7NeF3.png</t>
-  </si>
-  <si>
-    <t>https://i.imgur.com/sclH3wO.png</t>
-  </si>
-  <si>
-    <t>https://i.imgur.com/Ay0SsXe.png</t>
-  </si>
-  <si>
-    <t>https://i.imgur.com/OwL8OBA.png</t>
-  </si>
-  <si>
-    <t>https://i.imgur.com/ARsYA1K.png</t>
-  </si>
-  <si>
-    <t>https://i.imgur.com/G0MNOx2.png</t>
-  </si>
-  <si>
-    <t>https://i.imgur.com/JtJYtkX.jpg</t>
-  </si>
-  <si>
-    <t>https://i.imgur.com/xKONxAZ.png</t>
-  </si>
-  <si>
-    <t>https://i.imgur.com/mQrejMN.jpg</t>
-  </si>
-  <si>
     <t>https://i.imgur.com/ADe5L3X.jpg</t>
-  </si>
-  <si>
-    <t>Prenda_Vestido_camisero_Vestido_camisero_Blanco_P01_seed4275</t>
-  </si>
-  <si>
-    <t>Prenda_Pantalón_palazzo_Pantalón_palazzo_Blanco_P02_seed6692</t>
-  </si>
-  <si>
-    <t>Prenda_Top_Top_Negro_P03_seed4206</t>
-  </si>
-  <si>
-    <t>Prenda_Falda_midi_satinada_Falda_midi_satinada_Gris_claro_P04_seed2216</t>
-  </si>
-  <si>
-    <t>Prenda_Falda_midi_satinada_Falda_midi_satinada_verde_P05_seed7292</t>
-  </si>
-  <si>
-    <t>Prenda_Chaqueta_Chaqueta_de_estilo_Elegante_en_color_Camel_P06_seed1474</t>
-  </si>
-  <si>
-    <t>Prenda_Polo_Polo_de_estilo_Elegante_en_color_Azul_P07_seed9180</t>
-  </si>
-  <si>
-    <t>Prenda_Camisa_Camisa_de_estilo_Casual_en_color_Beige_P08_seed8912</t>
-  </si>
-  <si>
-    <t>Prenda_Camiseta_Camiseta_blanca_P09_seed5276</t>
-  </si>
-  <si>
-    <t>Prenda_Chaqueta_Chaqueta_de_estilo_elegante_ceñida_Azul_marino_P10_seed3580</t>
-  </si>
-  <si>
-    <t>Prenda_Chaqueta_Chaqueta_vaquera_P11 _seed3547</t>
-  </si>
-  <si>
-    <t>Prenda_Pantalón_Pantalón_P12_seed5786</t>
-  </si>
-  <si>
-    <t>Prenda_Vaquero_Pantalón_P13_seed3420</t>
-  </si>
-  <si>
-    <t>Prenda_Sudadera_Sudadera_P14_seed7474</t>
-  </si>
-  <si>
-    <t>Prenda_Vestido_Vestido_rojo_P15_seed9029</t>
-  </si>
-  <si>
-    <t>Prenda_Camisa_Camisa_Blanca_P16_seed4304</t>
-  </si>
-  <si>
-    <t>Prenda_Camisa_Camisa_marrón_P17_seed8562</t>
-  </si>
-  <si>
-    <t>Prenda_Pantalón_Pantalón_Chino_azul_P18_seed1907</t>
-  </si>
-  <si>
-    <t>Prenda_Abrigo_Abrigo_Largo_verde_P19_seed6232</t>
   </si>
   <si>
     <t>Prenda_Pantalón_Pantalón_verde_P20_seed3821</t>
@@ -758,9 +775,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
   <fonts count="3">
     <font>
@@ -834,18 +851,26 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -883,7 +908,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -917,6 +942,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -951,9 +977,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1126,7 +1153,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -1200,13 +1227,13 @@
         <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="C2" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="D2" t="s">
-        <v>50</v>
+        <v>23</v>
       </c>
       <c r="E2" s="2">
         <v>32150</v>
@@ -1215,31 +1242,31 @@
         <v>37</v>
       </c>
       <c r="G2" t="s">
-        <v>52</v>
+        <v>24</v>
       </c>
       <c r="H2" t="s">
-        <v>62</v>
+        <v>25</v>
       </c>
       <c r="I2" t="s">
-        <v>71</v>
+        <v>26</v>
       </c>
       <c r="J2" t="s">
-        <v>77</v>
+        <v>27</v>
       </c>
       <c r="K2">
         <v>8821</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>81</v>
+        <v>28</v>
       </c>
       <c r="M2" t="s">
-        <v>91</v>
+        <v>29</v>
       </c>
       <c r="N2" t="s">
-        <v>97</v>
+        <v>30</v>
       </c>
       <c r="O2" t="s">
-        <v>99</v>
+        <v>31</v>
       </c>
       <c r="P2">
         <v>51.62</v>
@@ -1248,27 +1275,27 @@
         <v>45703</v>
       </c>
       <c r="R2" t="s">
-        <v>78</v>
+        <v>32</v>
       </c>
       <c r="S2" t="s">
-        <v>106</v>
+        <v>33</v>
       </c>
       <c r="T2" t="s">
-        <v>110</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:20">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="C3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D3" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="E3" s="2">
         <v>33381</v>
@@ -1277,31 +1304,31 @@
         <v>33</v>
       </c>
       <c r="G3" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="H3" t="s">
-        <v>63</v>
+        <v>40</v>
       </c>
       <c r="I3" t="s">
-        <v>72</v>
+        <v>41</v>
       </c>
       <c r="J3" t="s">
-        <v>78</v>
+        <v>32</v>
       </c>
       <c r="K3">
         <v>1160</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>82</v>
+        <v>42</v>
       </c>
       <c r="M3" t="s">
-        <v>92</v>
+        <v>43</v>
       </c>
       <c r="N3" t="s">
-        <v>98</v>
+        <v>44</v>
       </c>
       <c r="O3" t="s">
-        <v>99</v>
+        <v>31</v>
       </c>
       <c r="P3">
         <v>64</v>
@@ -1310,27 +1337,27 @@
         <v>45696</v>
       </c>
       <c r="R3" t="s">
-        <v>79</v>
+        <v>45</v>
       </c>
       <c r="S3" t="s">
-        <v>106</v>
+        <v>33</v>
       </c>
       <c r="T3" t="s">
-        <v>111</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:20">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>47</v>
       </c>
       <c r="B4" t="s">
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="C4" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="D4" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="E4" s="2">
         <v>30530</v>
@@ -1339,31 +1366,31 @@
         <v>41</v>
       </c>
       <c r="G4" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="H4" t="s">
-        <v>62</v>
+        <v>25</v>
       </c>
       <c r="I4" t="s">
-        <v>73</v>
+        <v>51</v>
       </c>
       <c r="J4" t="s">
-        <v>78</v>
+        <v>32</v>
       </c>
       <c r="K4">
         <v>7815</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>83</v>
+        <v>52</v>
       </c>
       <c r="M4" t="s">
-        <v>92</v>
+        <v>43</v>
       </c>
       <c r="N4" t="s">
-        <v>98</v>
+        <v>44</v>
       </c>
       <c r="O4" t="s">
-        <v>100</v>
+        <v>53</v>
       </c>
       <c r="P4">
         <v>60</v>
@@ -1372,27 +1399,27 @@
         <v>45686</v>
       </c>
       <c r="R4" t="s">
-        <v>77</v>
+        <v>27</v>
       </c>
       <c r="S4" t="s">
-        <v>107</v>
+        <v>54</v>
       </c>
       <c r="T4" t="s">
-        <v>112</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:20">
       <c r="A5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D5" t="s">
         <v>23</v>
-      </c>
-      <c r="B5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C5" t="s">
-        <v>43</v>
-      </c>
-      <c r="D5" t="s">
-        <v>50</v>
       </c>
       <c r="E5" s="2">
         <v>30163</v>
@@ -1401,31 +1428,31 @@
         <v>42</v>
       </c>
       <c r="G5" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="H5" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="I5" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="J5" t="s">
-        <v>79</v>
+        <v>45</v>
       </c>
       <c r="K5">
         <v>2402</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>84</v>
+        <v>62</v>
       </c>
       <c r="M5" t="s">
-        <v>93</v>
+        <v>63</v>
       </c>
       <c r="N5" t="s">
-        <v>97</v>
+        <v>30</v>
       </c>
       <c r="O5" t="s">
-        <v>101</v>
+        <v>64</v>
       </c>
       <c r="P5">
         <v>45</v>
@@ -1434,27 +1461,27 @@
         <v>45675</v>
       </c>
       <c r="R5" t="s">
-        <v>79</v>
+        <v>45</v>
       </c>
       <c r="S5" t="s">
-        <v>108</v>
+        <v>65</v>
       </c>
       <c r="T5" t="s">
-        <v>113</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:20">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>67</v>
       </c>
       <c r="B6" t="s">
-        <v>34</v>
+        <v>68</v>
       </c>
       <c r="C6" t="s">
-        <v>44</v>
+        <v>69</v>
       </c>
       <c r="D6" t="s">
-        <v>50</v>
+        <v>23</v>
       </c>
       <c r="E6" s="2">
         <v>31940</v>
@@ -1463,31 +1490,31 @@
         <v>37</v>
       </c>
       <c r="G6" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="H6" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="I6" t="s">
-        <v>73</v>
+        <v>51</v>
       </c>
       <c r="J6" t="s">
-        <v>79</v>
+        <v>45</v>
       </c>
       <c r="K6">
         <v>3079</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="M6" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="N6" t="s">
-        <v>97</v>
+        <v>30</v>
       </c>
       <c r="O6" t="s">
-        <v>102</v>
+        <v>74</v>
       </c>
       <c r="P6">
         <v>55</v>
@@ -1496,27 +1523,27 @@
         <v>45708</v>
       </c>
       <c r="R6" t="s">
-        <v>79</v>
+        <v>45</v>
       </c>
       <c r="S6" t="s">
-        <v>109</v>
+        <v>75</v>
       </c>
       <c r="T6" t="s">
-        <v>114</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:20">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>77</v>
       </c>
       <c r="B7" t="s">
-        <v>35</v>
+        <v>78</v>
       </c>
       <c r="C7" t="s">
-        <v>45</v>
+        <v>79</v>
       </c>
       <c r="D7" t="s">
-        <v>50</v>
+        <v>23</v>
       </c>
       <c r="E7" s="2">
         <v>32420</v>
@@ -1525,31 +1552,31 @@
         <v>36</v>
       </c>
       <c r="G7" t="s">
-        <v>57</v>
+        <v>80</v>
       </c>
       <c r="H7" t="s">
-        <v>66</v>
+        <v>81</v>
       </c>
       <c r="I7" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="J7" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="K7">
         <v>6037</v>
       </c>
       <c r="L7" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="M7" t="s">
+        <v>85</v>
+      </c>
+      <c r="N7" t="s">
+        <v>30</v>
+      </c>
+      <c r="O7" t="s">
         <v>86</v>
-      </c>
-      <c r="M7" t="s">
-        <v>95</v>
-      </c>
-      <c r="N7" t="s">
-        <v>97</v>
-      </c>
-      <c r="O7" t="s">
-        <v>103</v>
       </c>
       <c r="P7">
         <v>60</v>
@@ -1558,24 +1585,24 @@
         <v>45576</v>
       </c>
       <c r="R7" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="T7" t="s">
-        <v>115</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:20">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>88</v>
       </c>
       <c r="B8" t="s">
-        <v>36</v>
+        <v>89</v>
       </c>
       <c r="C8" t="s">
-        <v>46</v>
+        <v>90</v>
       </c>
       <c r="D8" t="s">
-        <v>50</v>
+        <v>23</v>
       </c>
       <c r="E8" s="2">
         <v>34279</v>
@@ -1584,31 +1611,31 @@
         <v>31</v>
       </c>
       <c r="G8" t="s">
-        <v>58</v>
+        <v>91</v>
       </c>
       <c r="H8" t="s">
-        <v>67</v>
+        <v>92</v>
       </c>
       <c r="I8" t="s">
-        <v>76</v>
+        <v>93</v>
       </c>
       <c r="J8" t="s">
-        <v>77</v>
+        <v>27</v>
       </c>
       <c r="K8">
         <v>8723</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="M8" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="N8" t="s">
-        <v>97</v>
+        <v>30</v>
       </c>
       <c r="O8" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="P8">
         <v>80</v>
@@ -1617,24 +1644,24 @@
         <v>45641</v>
       </c>
       <c r="R8" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="T8" t="s">
-        <v>116</v>
+        <v>97</v>
       </c>
     </row>
     <row r="9" spans="1:20">
       <c r="A9" t="s">
-        <v>27</v>
+        <v>98</v>
       </c>
       <c r="B9" t="s">
-        <v>37</v>
+        <v>99</v>
       </c>
       <c r="C9" t="s">
-        <v>47</v>
+        <v>100</v>
       </c>
       <c r="D9" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="E9" s="2">
         <v>35754</v>
@@ -1643,31 +1670,31 @@
         <v>27</v>
       </c>
       <c r="G9" t="s">
-        <v>59</v>
+        <v>101</v>
       </c>
       <c r="H9" t="s">
-        <v>68</v>
+        <v>102</v>
       </c>
       <c r="I9" t="s">
-        <v>73</v>
+        <v>51</v>
       </c>
       <c r="J9" t="s">
-        <v>79</v>
+        <v>45</v>
       </c>
       <c r="K9">
         <v>8821</v>
       </c>
       <c r="L9" s="3" t="s">
-        <v>88</v>
+        <v>103</v>
       </c>
       <c r="M9" t="s">
-        <v>93</v>
+        <v>63</v>
       </c>
       <c r="N9" t="s">
-        <v>97</v>
+        <v>30</v>
       </c>
       <c r="O9" t="s">
-        <v>101</v>
+        <v>64</v>
       </c>
       <c r="P9">
         <v>80</v>
@@ -1676,27 +1703,27 @@
         <v>45608</v>
       </c>
       <c r="R9" t="s">
-        <v>78</v>
+        <v>32</v>
       </c>
       <c r="S9" t="s">
-        <v>108</v>
+        <v>65</v>
       </c>
       <c r="T9" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
     </row>
     <row r="10" spans="1:20">
       <c r="A10" t="s">
-        <v>28</v>
+        <v>105</v>
       </c>
       <c r="B10" t="s">
+        <v>106</v>
+      </c>
+      <c r="C10" t="s">
+        <v>107</v>
+      </c>
+      <c r="D10" t="s">
         <v>38</v>
-      </c>
-      <c r="C10" t="s">
-        <v>48</v>
-      </c>
-      <c r="D10" t="s">
-        <v>51</v>
       </c>
       <c r="E10" s="2">
         <v>24230</v>
@@ -1705,31 +1732,31 @@
         <v>48</v>
       </c>
       <c r="G10" t="s">
-        <v>60</v>
+        <v>108</v>
       </c>
       <c r="H10" t="s">
-        <v>69</v>
+        <v>109</v>
       </c>
       <c r="I10" t="s">
-        <v>72</v>
+        <v>41</v>
       </c>
       <c r="J10" t="s">
-        <v>79</v>
+        <v>45</v>
       </c>
       <c r="K10">
         <v>1817</v>
       </c>
       <c r="L10" s="3" t="s">
-        <v>89</v>
+        <v>110</v>
       </c>
       <c r="M10" t="s">
-        <v>91</v>
+        <v>29</v>
       </c>
       <c r="N10" t="s">
-        <v>97</v>
+        <v>30</v>
       </c>
       <c r="O10" t="s">
-        <v>100</v>
+        <v>53</v>
       </c>
       <c r="P10">
         <v>65</v>
@@ -1738,27 +1765,27 @@
         <v>45586</v>
       </c>
       <c r="R10" t="s">
-        <v>79</v>
+        <v>45</v>
       </c>
       <c r="S10" t="s">
-        <v>107</v>
+        <v>54</v>
       </c>
       <c r="T10" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
     </row>
     <row r="11" spans="1:20">
       <c r="A11" t="s">
-        <v>29</v>
+        <v>112</v>
       </c>
       <c r="B11" t="s">
-        <v>39</v>
+        <v>113</v>
       </c>
       <c r="C11" t="s">
-        <v>49</v>
+        <v>114</v>
       </c>
       <c r="D11" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="E11" s="2">
         <v>27131</v>
@@ -1767,31 +1794,31 @@
         <v>50</v>
       </c>
       <c r="G11" t="s">
-        <v>61</v>
+        <v>115</v>
       </c>
       <c r="H11" t="s">
-        <v>70</v>
+        <v>116</v>
       </c>
       <c r="I11" t="s">
-        <v>72</v>
+        <v>41</v>
       </c>
       <c r="J11" t="s">
-        <v>78</v>
+        <v>32</v>
       </c>
       <c r="K11">
         <v>6053</v>
       </c>
       <c r="L11" s="3" t="s">
-        <v>90</v>
+        <v>117</v>
       </c>
       <c r="M11" t="s">
-        <v>96</v>
+        <v>118</v>
       </c>
       <c r="N11" t="s">
-        <v>97</v>
+        <v>30</v>
       </c>
       <c r="O11" t="s">
-        <v>102</v>
+        <v>74</v>
       </c>
       <c r="P11">
         <v>65</v>
@@ -1800,10 +1827,10 @@
         <v>45674</v>
       </c>
       <c r="R11" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="S11" t="s">
-        <v>109</v>
+        <v>75</v>
       </c>
       <c r="T11" t="s">
         <v>119</v>
@@ -1811,23 +1838,23 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="L2" r:id="rId1"/>
-    <hyperlink ref="L3" r:id="rId2"/>
-    <hyperlink ref="L4" r:id="rId3"/>
-    <hyperlink ref="L5" r:id="rId4"/>
-    <hyperlink ref="L6" r:id="rId5"/>
-    <hyperlink ref="L7" r:id="rId6"/>
-    <hyperlink ref="L8" r:id="rId7"/>
-    <hyperlink ref="L9" r:id="rId8"/>
-    <hyperlink ref="L10" r:id="rId9"/>
-    <hyperlink ref="L11" r:id="rId10"/>
+    <hyperlink ref="L2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="L3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="L4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="L5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="L6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="L7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="L8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="L9" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="L10" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="L11" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:O21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1886,936 +1913,936 @@
         <v>132</v>
       </c>
       <c r="B2" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
       <c r="C2" t="s">
-        <v>167</v>
+        <v>134</v>
       </c>
       <c r="D2" t="s">
-        <v>177</v>
+        <v>135</v>
       </c>
       <c r="E2" t="s">
-        <v>50</v>
+        <v>23</v>
       </c>
       <c r="F2" t="s">
-        <v>71</v>
+        <v>26</v>
       </c>
       <c r="G2" t="s">
-        <v>185</v>
+        <v>136</v>
       </c>
       <c r="H2" t="s">
-        <v>190</v>
+        <v>137</v>
       </c>
       <c r="I2" t="s">
-        <v>91</v>
+        <v>29</v>
       </c>
       <c r="J2">
         <v>51.62</v>
       </c>
       <c r="K2" t="s">
-        <v>194</v>
+        <v>138</v>
       </c>
       <c r="L2" t="s">
-        <v>197</v>
+        <v>139</v>
       </c>
       <c r="M2">
         <v>4275</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>206</v>
+        <v>140</v>
       </c>
       <c r="O2" t="s">
-        <v>226</v>
+        <v>141</v>
       </c>
     </row>
     <row r="3" spans="1:15">
       <c r="A3" t="s">
-        <v>133</v>
+        <v>142</v>
       </c>
       <c r="B3" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="C3" t="s">
-        <v>168</v>
+        <v>144</v>
       </c>
       <c r="D3" t="s">
-        <v>177</v>
+        <v>135</v>
       </c>
       <c r="E3" t="s">
-        <v>50</v>
+        <v>23</v>
       </c>
       <c r="F3" t="s">
-        <v>71</v>
+        <v>26</v>
       </c>
       <c r="G3" t="s">
-        <v>185</v>
+        <v>136</v>
       </c>
       <c r="H3" t="s">
-        <v>190</v>
+        <v>137</v>
       </c>
       <c r="I3" t="s">
-        <v>91</v>
+        <v>29</v>
       </c>
       <c r="J3">
         <v>51.62</v>
       </c>
       <c r="K3" t="s">
-        <v>194</v>
+        <v>138</v>
       </c>
       <c r="L3" t="s">
-        <v>197</v>
+        <v>139</v>
       </c>
       <c r="M3">
         <v>6692</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>207</v>
+        <v>145</v>
       </c>
       <c r="O3" t="s">
-        <v>227</v>
+        <v>146</v>
       </c>
     </row>
     <row r="4" spans="1:15">
       <c r="A4" t="s">
-        <v>134</v>
+        <v>147</v>
       </c>
       <c r="B4" t="s">
+        <v>148</v>
+      </c>
+      <c r="C4" t="s">
+        <v>149</v>
+      </c>
+      <c r="D4" t="s">
+        <v>149</v>
+      </c>
+      <c r="E4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" t="s">
+        <v>51</v>
+      </c>
+      <c r="G4" t="s">
         <v>150</v>
       </c>
-      <c r="C4" t="s">
-        <v>169</v>
-      </c>
-      <c r="D4" t="s">
-        <v>169</v>
-      </c>
-      <c r="E4" t="s">
-        <v>50</v>
-      </c>
-      <c r="F4" t="s">
-        <v>73</v>
-      </c>
-      <c r="G4" t="s">
-        <v>186</v>
-      </c>
       <c r="H4" t="s">
-        <v>191</v>
+        <v>151</v>
       </c>
       <c r="I4" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="J4">
         <v>50.69</v>
       </c>
       <c r="K4" t="s">
-        <v>195</v>
+        <v>152</v>
       </c>
       <c r="L4" t="s">
-        <v>198</v>
+        <v>153</v>
       </c>
       <c r="M4">
         <v>4206</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>208</v>
+        <v>154</v>
       </c>
       <c r="O4" t="s">
-        <v>228</v>
+        <v>155</v>
       </c>
     </row>
     <row r="5" spans="1:15">
       <c r="A5" t="s">
-        <v>135</v>
+        <v>156</v>
       </c>
       <c r="B5" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="C5" t="s">
-        <v>170</v>
+        <v>158</v>
       </c>
       <c r="D5" t="s">
-        <v>179</v>
+        <v>159</v>
       </c>
       <c r="E5" t="s">
-        <v>50</v>
+        <v>23</v>
       </c>
       <c r="F5" t="s">
-        <v>71</v>
+        <v>26</v>
       </c>
       <c r="G5" t="s">
-        <v>187</v>
+        <v>160</v>
       </c>
       <c r="H5" t="s">
-        <v>190</v>
+        <v>137</v>
       </c>
       <c r="I5" t="s">
-        <v>193</v>
+        <v>161</v>
       </c>
       <c r="J5">
         <v>110.65</v>
       </c>
       <c r="K5" t="s">
-        <v>195</v>
+        <v>152</v>
       </c>
       <c r="L5" t="s">
-        <v>199</v>
+        <v>162</v>
       </c>
       <c r="M5">
         <v>2216</v>
       </c>
       <c r="N5" s="3" t="s">
-        <v>209</v>
+        <v>163</v>
       </c>
       <c r="O5" t="s">
-        <v>229</v>
+        <v>164</v>
       </c>
     </row>
     <row r="6" spans="1:15">
       <c r="A6" t="s">
-        <v>136</v>
+        <v>165</v>
       </c>
       <c r="B6" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="C6" t="s">
-        <v>170</v>
+        <v>158</v>
       </c>
       <c r="D6" t="s">
-        <v>179</v>
+        <v>159</v>
       </c>
       <c r="E6" t="s">
-        <v>50</v>
+        <v>23</v>
       </c>
       <c r="F6" t="s">
-        <v>184</v>
+        <v>167</v>
       </c>
       <c r="G6" t="s">
-        <v>186</v>
+        <v>150</v>
       </c>
       <c r="H6" t="s">
-        <v>192</v>
+        <v>168</v>
       </c>
       <c r="I6" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="J6">
         <v>38.5</v>
       </c>
       <c r="K6" t="s">
-        <v>194</v>
+        <v>138</v>
       </c>
       <c r="L6" t="s">
-        <v>200</v>
+        <v>169</v>
       </c>
       <c r="M6">
         <v>7292</v>
       </c>
       <c r="N6" s="3" t="s">
-        <v>210</v>
+        <v>170</v>
       </c>
       <c r="O6" t="s">
-        <v>230</v>
+        <v>171</v>
       </c>
     </row>
     <row r="7" spans="1:15">
       <c r="A7" t="s">
-        <v>106</v>
+        <v>33</v>
       </c>
       <c r="B7" t="s">
-        <v>153</v>
+        <v>172</v>
       </c>
       <c r="C7" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="D7" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="E7" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="F7" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="G7" t="s">
-        <v>185</v>
+        <v>136</v>
       </c>
       <c r="H7" t="s">
-        <v>192</v>
+        <v>168</v>
       </c>
       <c r="I7" t="s">
-        <v>91</v>
+        <v>29</v>
       </c>
       <c r="J7">
         <v>150</v>
       </c>
       <c r="K7" t="s">
-        <v>196</v>
+        <v>174</v>
       </c>
       <c r="L7" t="s">
-        <v>201</v>
+        <v>175</v>
       </c>
       <c r="M7">
         <v>1474</v>
       </c>
       <c r="N7" s="3" t="s">
-        <v>211</v>
+        <v>176</v>
       </c>
       <c r="O7" t="s">
-        <v>231</v>
+        <v>177</v>
       </c>
     </row>
     <row r="8" spans="1:15">
       <c r="A8" t="s">
-        <v>137</v>
+        <v>178</v>
       </c>
       <c r="B8" t="s">
-        <v>154</v>
+        <v>179</v>
       </c>
       <c r="C8" t="s">
-        <v>172</v>
+        <v>180</v>
       </c>
       <c r="D8" t="s">
-        <v>172</v>
+        <v>180</v>
       </c>
       <c r="E8" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="F8" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="G8" t="s">
-        <v>187</v>
+        <v>160</v>
       </c>
       <c r="H8" t="s">
-        <v>192</v>
+        <v>168</v>
       </c>
       <c r="I8" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="J8">
         <v>85</v>
       </c>
       <c r="K8" t="s">
-        <v>195</v>
+        <v>152</v>
       </c>
       <c r="L8" t="s">
-        <v>202</v>
+        <v>181</v>
       </c>
       <c r="M8">
         <v>9180</v>
       </c>
       <c r="N8" s="3" t="s">
-        <v>212</v>
+        <v>182</v>
       </c>
       <c r="O8" t="s">
-        <v>232</v>
+        <v>183</v>
       </c>
     </row>
     <row r="9" spans="1:15">
       <c r="A9" t="s">
-        <v>138</v>
+        <v>184</v>
       </c>
       <c r="B9" t="s">
-        <v>155</v>
+        <v>185</v>
       </c>
       <c r="C9" t="s">
-        <v>173</v>
+        <v>186</v>
       </c>
       <c r="D9" t="s">
-        <v>173</v>
+        <v>186</v>
       </c>
       <c r="E9" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="F9" t="s">
-        <v>184</v>
+        <v>167</v>
       </c>
       <c r="G9" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="H9" t="s">
-        <v>190</v>
+        <v>137</v>
       </c>
       <c r="I9" t="s">
-        <v>184</v>
+        <v>167</v>
       </c>
       <c r="J9">
         <v>60</v>
       </c>
       <c r="K9" t="s">
-        <v>194</v>
+        <v>138</v>
       </c>
       <c r="L9" t="s">
-        <v>203</v>
+        <v>188</v>
       </c>
       <c r="M9">
         <v>8912</v>
       </c>
       <c r="N9" s="3" t="s">
-        <v>213</v>
+        <v>189</v>
       </c>
       <c r="O9" t="s">
-        <v>233</v>
+        <v>190</v>
       </c>
     </row>
     <row r="10" spans="1:15">
       <c r="A10" t="s">
-        <v>108</v>
+        <v>65</v>
       </c>
       <c r="B10" t="s">
-        <v>156</v>
+        <v>191</v>
       </c>
       <c r="C10" t="s">
-        <v>174</v>
+        <v>192</v>
       </c>
       <c r="D10" t="s">
-        <v>174</v>
+        <v>192</v>
       </c>
       <c r="E10" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="F10" t="s">
-        <v>184</v>
+        <v>167</v>
       </c>
       <c r="G10" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="H10" t="s">
-        <v>190</v>
+        <v>137</v>
       </c>
       <c r="I10" t="s">
-        <v>184</v>
+        <v>167</v>
       </c>
       <c r="J10">
         <v>25</v>
       </c>
       <c r="K10" t="s">
+        <v>138</v>
+      </c>
+      <c r="L10" t="s">
         <v>194</v>
-      </c>
-      <c r="L10" t="s">
-        <v>204</v>
       </c>
       <c r="M10">
         <v>5276</v>
       </c>
       <c r="N10" s="3" t="s">
-        <v>214</v>
+        <v>195</v>
       </c>
       <c r="O10" t="s">
-        <v>234</v>
+        <v>196</v>
       </c>
     </row>
     <row r="11" spans="1:15">
       <c r="A11" t="s">
-        <v>139</v>
+        <v>197</v>
       </c>
       <c r="B11" t="s">
-        <v>157</v>
+        <v>198</v>
       </c>
       <c r="C11" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="D11" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="E11" t="s">
-        <v>50</v>
+        <v>23</v>
       </c>
       <c r="F11" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="G11" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="H11" t="s">
-        <v>192</v>
+        <v>168</v>
       </c>
       <c r="I11" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="J11">
         <v>180</v>
       </c>
       <c r="K11" t="s">
-        <v>195</v>
+        <v>152</v>
       </c>
       <c r="L11" t="s">
-        <v>202</v>
+        <v>181</v>
       </c>
       <c r="M11">
         <v>3580</v>
       </c>
       <c r="N11" s="3" t="s">
-        <v>215</v>
+        <v>199</v>
       </c>
       <c r="O11" t="s">
-        <v>235</v>
+        <v>200</v>
       </c>
     </row>
     <row r="12" spans="1:15">
       <c r="A12" t="s">
-        <v>140</v>
+        <v>201</v>
       </c>
       <c r="B12" t="s">
-        <v>158</v>
+        <v>202</v>
       </c>
       <c r="C12" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="D12" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="E12" t="s">
-        <v>50</v>
+        <v>23</v>
       </c>
       <c r="F12" t="s">
-        <v>184</v>
+        <v>167</v>
       </c>
       <c r="G12" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="H12" t="s">
-        <v>192</v>
+        <v>168</v>
       </c>
       <c r="I12" t="s">
-        <v>184</v>
+        <v>167</v>
       </c>
       <c r="J12">
         <v>69</v>
       </c>
       <c r="K12" t="s">
-        <v>194</v>
+        <v>138</v>
       </c>
       <c r="L12" t="s">
-        <v>202</v>
+        <v>181</v>
       </c>
       <c r="M12">
         <v>3547</v>
       </c>
       <c r="N12" s="3" t="s">
-        <v>216</v>
+        <v>203</v>
       </c>
       <c r="O12" t="s">
-        <v>236</v>
+        <v>204</v>
       </c>
     </row>
     <row r="13" spans="1:15">
       <c r="A13" t="s">
-        <v>141</v>
+        <v>205</v>
       </c>
       <c r="B13" t="s">
-        <v>159</v>
+        <v>206</v>
       </c>
       <c r="C13" t="s">
-        <v>175</v>
+        <v>207</v>
       </c>
       <c r="D13" t="s">
-        <v>180</v>
+        <v>208</v>
       </c>
       <c r="E13" t="s">
-        <v>50</v>
+        <v>23</v>
       </c>
       <c r="F13" t="s">
-        <v>184</v>
+        <v>167</v>
       </c>
       <c r="G13" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="H13" t="s">
-        <v>190</v>
+        <v>137</v>
       </c>
       <c r="I13" t="s">
-        <v>184</v>
+        <v>167</v>
       </c>
       <c r="J13">
         <v>25</v>
       </c>
       <c r="K13" t="s">
+        <v>138</v>
+      </c>
+      <c r="L13" t="s">
         <v>194</v>
-      </c>
-      <c r="L13" t="s">
-        <v>204</v>
       </c>
       <c r="M13">
         <v>5786</v>
       </c>
       <c r="N13" s="3" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="O13" t="s">
-        <v>237</v>
+        <v>210</v>
       </c>
     </row>
     <row r="14" spans="1:15">
       <c r="A14" t="s">
-        <v>142</v>
+        <v>211</v>
       </c>
       <c r="B14" t="s">
-        <v>159</v>
+        <v>206</v>
       </c>
       <c r="C14" t="s">
-        <v>176</v>
+        <v>212</v>
       </c>
       <c r="D14" t="s">
-        <v>181</v>
+        <v>213</v>
       </c>
       <c r="E14" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="F14" t="s">
-        <v>184</v>
+        <v>167</v>
       </c>
       <c r="G14" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="H14" t="s">
-        <v>190</v>
+        <v>137</v>
       </c>
       <c r="I14" t="s">
-        <v>184</v>
+        <v>167</v>
       </c>
       <c r="J14">
         <v>85</v>
       </c>
       <c r="K14" t="s">
-        <v>195</v>
+        <v>152</v>
       </c>
       <c r="L14" t="s">
-        <v>202</v>
+        <v>181</v>
       </c>
       <c r="M14">
         <v>3420</v>
       </c>
       <c r="N14" s="3" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="O14" t="s">
-        <v>238</v>
+        <v>215</v>
       </c>
     </row>
     <row r="15" spans="1:15">
       <c r="A15" t="s">
-        <v>109</v>
+        <v>75</v>
       </c>
       <c r="B15" t="s">
-        <v>160</v>
+        <v>216</v>
       </c>
       <c r="C15" t="s">
-        <v>160</v>
+        <v>216</v>
       </c>
       <c r="D15" t="s">
-        <v>181</v>
+        <v>213</v>
       </c>
       <c r="E15" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="F15" t="s">
-        <v>184</v>
+        <v>167</v>
       </c>
       <c r="G15" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="H15" t="s">
-        <v>190</v>
+        <v>137</v>
       </c>
       <c r="I15" t="s">
-        <v>184</v>
+        <v>167</v>
       </c>
       <c r="J15">
         <v>50</v>
       </c>
       <c r="K15" t="s">
-        <v>195</v>
+        <v>152</v>
       </c>
       <c r="L15" t="s">
-        <v>202</v>
+        <v>181</v>
       </c>
       <c r="M15">
         <v>7474</v>
       </c>
       <c r="N15" s="3" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="O15" t="s">
-        <v>239</v>
+        <v>218</v>
       </c>
     </row>
     <row r="16" spans="1:15">
       <c r="A16" t="s">
-        <v>143</v>
+        <v>219</v>
       </c>
       <c r="B16" t="s">
+        <v>220</v>
+      </c>
+      <c r="C16" t="s">
+        <v>135</v>
+      </c>
+      <c r="D16" t="s">
+        <v>82</v>
+      </c>
+      <c r="E16" t="s">
+        <v>23</v>
+      </c>
+      <c r="F16" t="s">
+        <v>82</v>
+      </c>
+      <c r="G16" t="s">
+        <v>160</v>
+      </c>
+      <c r="H16" t="s">
+        <v>137</v>
+      </c>
+      <c r="I16" t="s">
         <v>161</v>
-      </c>
-      <c r="C16" t="s">
-        <v>177</v>
-      </c>
-      <c r="D16" t="s">
-        <v>75</v>
-      </c>
-      <c r="E16" t="s">
-        <v>50</v>
-      </c>
-      <c r="F16" t="s">
-        <v>75</v>
-      </c>
-      <c r="G16" t="s">
-        <v>187</v>
-      </c>
-      <c r="H16" t="s">
-        <v>190</v>
-      </c>
-      <c r="I16" t="s">
-        <v>193</v>
       </c>
       <c r="J16">
         <v>150</v>
       </c>
       <c r="K16" t="s">
-        <v>196</v>
+        <v>174</v>
       </c>
       <c r="L16" t="s">
-        <v>199</v>
+        <v>162</v>
       </c>
       <c r="M16">
         <v>9029</v>
       </c>
       <c r="N16" s="3" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="O16" t="s">
-        <v>240</v>
+        <v>222</v>
       </c>
     </row>
     <row r="17" spans="1:15">
       <c r="A17" t="s">
-        <v>144</v>
+        <v>223</v>
       </c>
       <c r="B17" t="s">
-        <v>162</v>
+        <v>224</v>
       </c>
       <c r="C17" t="s">
-        <v>173</v>
+        <v>186</v>
       </c>
       <c r="D17" t="s">
-        <v>182</v>
+        <v>225</v>
       </c>
       <c r="E17" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="F17" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="G17" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="H17" t="s">
-        <v>190</v>
+        <v>137</v>
       </c>
       <c r="I17" t="s">
-        <v>96</v>
+        <v>118</v>
       </c>
       <c r="J17">
         <v>100</v>
       </c>
       <c r="K17" t="s">
-        <v>195</v>
+        <v>152</v>
       </c>
       <c r="L17" t="s">
-        <v>205</v>
+        <v>226</v>
       </c>
       <c r="M17">
         <v>4304</v>
       </c>
       <c r="N17" s="3" t="s">
-        <v>221</v>
+        <v>227</v>
       </c>
       <c r="O17" t="s">
-        <v>241</v>
+        <v>228</v>
       </c>
     </row>
     <row r="18" spans="1:15">
       <c r="A18" t="s">
-        <v>107</v>
+        <v>54</v>
       </c>
       <c r="B18" t="s">
-        <v>163</v>
+        <v>229</v>
       </c>
       <c r="C18" t="s">
-        <v>173</v>
+        <v>186</v>
       </c>
       <c r="D18" t="s">
-        <v>173</v>
+        <v>186</v>
       </c>
       <c r="E18" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="F18" t="s">
-        <v>184</v>
+        <v>167</v>
       </c>
       <c r="G18" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="H18" t="s">
-        <v>191</v>
+        <v>151</v>
       </c>
       <c r="I18" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="J18">
         <v>50</v>
       </c>
       <c r="K18" t="s">
-        <v>195</v>
+        <v>152</v>
       </c>
       <c r="L18" t="s">
-        <v>199</v>
+        <v>162</v>
       </c>
       <c r="M18">
         <v>8562</v>
       </c>
       <c r="N18" s="3" t="s">
-        <v>222</v>
+        <v>230</v>
       </c>
       <c r="O18" t="s">
-        <v>242</v>
+        <v>231</v>
       </c>
     </row>
     <row r="19" spans="1:15">
       <c r="A19" t="s">
-        <v>145</v>
+        <v>232</v>
       </c>
       <c r="B19" t="s">
-        <v>164</v>
+        <v>233</v>
       </c>
       <c r="C19" t="s">
-        <v>159</v>
+        <v>206</v>
       </c>
       <c r="D19" t="s">
-        <v>183</v>
+        <v>234</v>
       </c>
       <c r="E19" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="F19" t="s">
-        <v>184</v>
+        <v>167</v>
       </c>
       <c r="G19" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="H19" t="s">
-        <v>191</v>
+        <v>151</v>
       </c>
       <c r="I19" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="J19">
         <v>50</v>
       </c>
       <c r="K19" t="s">
-        <v>195</v>
+        <v>152</v>
       </c>
       <c r="L19" t="s">
-        <v>199</v>
+        <v>162</v>
       </c>
       <c r="M19">
         <v>1907</v>
       </c>
       <c r="N19" s="3" t="s">
-        <v>223</v>
+        <v>235</v>
       </c>
       <c r="O19" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
     </row>
     <row r="20" spans="1:15">
       <c r="A20" t="s">
-        <v>146</v>
+        <v>237</v>
       </c>
       <c r="B20" t="s">
-        <v>165</v>
+        <v>238</v>
       </c>
       <c r="C20" t="s">
-        <v>178</v>
+        <v>239</v>
       </c>
       <c r="D20" t="s">
-        <v>178</v>
+        <v>239</v>
       </c>
       <c r="E20" t="s">
-        <v>50</v>
+        <v>23</v>
       </c>
       <c r="F20" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="G20" t="s">
-        <v>186</v>
+        <v>150</v>
       </c>
       <c r="H20" t="s">
-        <v>192</v>
+        <v>168</v>
       </c>
       <c r="I20" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="J20">
         <v>180</v>
       </c>
       <c r="K20" t="s">
-        <v>195</v>
+        <v>152</v>
       </c>
       <c r="L20" t="s">
-        <v>200</v>
+        <v>169</v>
       </c>
       <c r="M20">
         <v>6232</v>
       </c>
       <c r="N20" s="3" t="s">
-        <v>224</v>
+        <v>240</v>
       </c>
       <c r="O20" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="21" spans="1:15">
       <c r="A21" t="s">
-        <v>147</v>
+        <v>242</v>
       </c>
       <c r="B21" t="s">
-        <v>166</v>
+        <v>243</v>
       </c>
       <c r="C21" t="s">
-        <v>159</v>
+        <v>206</v>
       </c>
       <c r="D21" t="s">
-        <v>159</v>
+        <v>206</v>
       </c>
       <c r="E21" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="F21" t="s">
-        <v>184</v>
+        <v>167</v>
       </c>
       <c r="G21" t="s">
-        <v>187</v>
+        <v>160</v>
       </c>
       <c r="H21" t="s">
-        <v>192</v>
+        <v>168</v>
       </c>
       <c r="I21" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="J21">
         <v>85</v>
       </c>
       <c r="K21" t="s">
-        <v>194</v>
+        <v>138</v>
       </c>
       <c r="L21" t="s">
-        <v>200</v>
+        <v>169</v>
       </c>
       <c r="M21">
         <v>3821</v>
       </c>
       <c r="N21" s="3" t="s">
-        <v>225</v>
+        <v>244</v>
       </c>
       <c r="O21" t="s">
         <v>245</v>
@@ -2823,26 +2850,26 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="N2" r:id="rId1"/>
-    <hyperlink ref="N3" r:id="rId2"/>
-    <hyperlink ref="N4" r:id="rId3"/>
-    <hyperlink ref="N5" r:id="rId4"/>
-    <hyperlink ref="N6" r:id="rId5"/>
-    <hyperlink ref="N7" r:id="rId6"/>
-    <hyperlink ref="N8" r:id="rId7"/>
-    <hyperlink ref="N9" r:id="rId8"/>
-    <hyperlink ref="N10" r:id="rId9"/>
-    <hyperlink ref="N11" r:id="rId10"/>
-    <hyperlink ref="N12" r:id="rId11"/>
-    <hyperlink ref="N13" r:id="rId12"/>
-    <hyperlink ref="N14" r:id="rId13"/>
-    <hyperlink ref="N15" r:id="rId14"/>
-    <hyperlink ref="N16" r:id="rId15"/>
-    <hyperlink ref="N17" r:id="rId16"/>
-    <hyperlink ref="N18" r:id="rId17"/>
-    <hyperlink ref="N19" r:id="rId18"/>
-    <hyperlink ref="N20" r:id="rId19"/>
-    <hyperlink ref="N21" r:id="rId20"/>
+    <hyperlink ref="N2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="N3" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="N4" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="N5" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="N6" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
+    <hyperlink ref="N7" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
+    <hyperlink ref="N8" r:id="rId7" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
+    <hyperlink ref="N9" r:id="rId8" xr:uid="{00000000-0004-0000-0100-000007000000}"/>
+    <hyperlink ref="N10" r:id="rId9" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
+    <hyperlink ref="N11" r:id="rId10" xr:uid="{00000000-0004-0000-0100-000009000000}"/>
+    <hyperlink ref="N12" r:id="rId11" xr:uid="{00000000-0004-0000-0100-00000A000000}"/>
+    <hyperlink ref="N13" r:id="rId12" xr:uid="{00000000-0004-0000-0100-00000B000000}"/>
+    <hyperlink ref="N14" r:id="rId13" xr:uid="{00000000-0004-0000-0100-00000C000000}"/>
+    <hyperlink ref="N15" r:id="rId14" xr:uid="{00000000-0004-0000-0100-00000D000000}"/>
+    <hyperlink ref="N16" r:id="rId15" xr:uid="{00000000-0004-0000-0100-00000E000000}"/>
+    <hyperlink ref="N17" r:id="rId16" xr:uid="{00000000-0004-0000-0100-00000F000000}"/>
+    <hyperlink ref="N18" r:id="rId17" xr:uid="{00000000-0004-0000-0100-000010000000}"/>
+    <hyperlink ref="N19" r:id="rId18" xr:uid="{00000000-0004-0000-0100-000011000000}"/>
+    <hyperlink ref="N20" r:id="rId19" xr:uid="{00000000-0004-0000-0100-000012000000}"/>
+    <hyperlink ref="N21" r:id="rId20" xr:uid="{00000000-0004-0000-0100-000013000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Corrijo nombre de columna Ciudad en hoja Avatares
</commit_message>
<xml_diff>
--- a/Base_Asistente_Imagenes_Estructuradas.xlsx
+++ b/Base_Asistente_Imagenes_Estructuradas.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28801"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{75FB986F-1C45-4DEA-A185-E8C09594A15C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{83649CF9-A224-4EC0-B185-E1540755A6D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -55,7 +55,7 @@
     <t>Email</t>
   </si>
   <si>
-    <t>Localidad</t>
+    <t>Ciudad</t>
   </si>
   <si>
     <t>Estilo preferido</t>
@@ -1156,9 +1156,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="30.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="19" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="42.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:20">
       <c r="A1" s="1" t="s">

</xml_diff>